<commit_message>
Fixed broken link to Asm Ref
</commit_message>
<xml_diff>
--- a/docs/materials/04-LanguageAbstractions/LA2-A-Assembly.xlsx
+++ b/docs/materials/04-LanguageAbstractions/LA2-A-Assembly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Spring23/COMP256/website/docs/materials/04-LanguageAbstractions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DC61DD-2BD8-D944-8CBF-2F350A629609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72E4E2F-FFAE-4841-A9BB-CBB7D2C925F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="760" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{6DDAC907-B27A-F447-A23B-697FDD4DA6D3}"/>
   </bookViews>
@@ -2683,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26F947F-27E6-AE4D-99A3-7DECFCCE924B}">
   <dimension ref="E1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:E48"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>